<commit_message>
Working version for  full album stats and user stats
</commit_message>
<xml_diff>
--- a/data/genres_list.xlsx
+++ b/data/genres_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/dev/rifftop/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F09CA4-1E26-EA4B-9F5D-3E87EE333761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0456C9C3-7937-F049-B028-F30158F2D744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="67">
   <si>
     <t>Heavy Metal</t>
   </si>
@@ -187,6 +187,51 @@
   </si>
   <si>
     <t>Prog Death Metal</t>
+  </si>
+  <si>
+    <t>genre</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>Doom</t>
+  </si>
+  <si>
+    <t>Prog &amp; Psychedelia</t>
+  </si>
+  <si>
+    <t>Tutoiement de l'Infini</t>
+  </si>
+  <si>
+    <t>Punk / Hardcore</t>
+  </si>
+  <si>
+    <t>Goths &amp; Corbacs</t>
+  </si>
+  <si>
+    <t>Indus</t>
+  </si>
+  <si>
+    <t>Folksies</t>
+  </si>
+  <si>
+    <t>Blues / Rock</t>
+  </si>
+  <si>
+    <t>Alternative / 90-2000s</t>
+  </si>
+  <si>
+    <t>Synthés</t>
+  </si>
+  <si>
+    <t>Avant-Garde &amp; Nawakeries</t>
+  </si>
+  <si>
+    <t>Americana</t>
+  </si>
+  <si>
+    <t>Stoner &amp; Desert Rock</t>
   </si>
 </sst>
 </file>
@@ -532,275 +577,448 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A52"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="235" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="235" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="B34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="B38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="B39" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="B40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="B41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="B42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="B43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="B45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="B46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="B48" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+      <c r="B49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+      <c r="B50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+      <c r="B52" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code cleanup. TODO : bug in user_stats::compute_score_weight
</commit_message>
<xml_diff>
--- a/data/genres_list.xlsx
+++ b/data/genres_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/dev/rifftop/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0456C9C3-7937-F049-B028-F30158F2D744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE2CB8C-F347-C84E-921B-EAC120DCAA86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32460" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="genres_list" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
   <si>
     <t>Heavy Metal</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Dark Synth - Dungeon synth</t>
   </si>
   <si>
-    <t>Post-Punk/Darkwave</t>
-  </si>
-  <si>
     <t>Fusion</t>
   </si>
   <si>
@@ -222,9 +219,6 @@
     <t>Alternative / 90-2000s</t>
   </si>
   <si>
-    <t>Synthés</t>
-  </si>
-  <si>
     <t>Avant-Garde &amp; Nawakeries</t>
   </si>
   <si>
@@ -232,6 +226,15 @@
   </si>
   <si>
     <t>Stoner &amp; Desert Rock</t>
+  </si>
+  <si>
+    <t>Goth / Darkwave</t>
+  </si>
+  <si>
+    <t>Post-Punk</t>
+  </si>
+  <si>
+    <t>Post-Punk / Indie Rock</t>
   </si>
 </sst>
 </file>
@@ -577,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="235" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="235" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -591,10 +594,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
         <v>52</v>
-      </c>
-      <c r="B1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -618,7 +621,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -642,7 +645,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -666,7 +669,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -674,7 +677,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -682,7 +685,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -690,7 +693,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -698,7 +701,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -706,7 +709,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -714,7 +717,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -722,7 +725,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -730,7 +733,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -738,7 +741,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -746,7 +749,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -754,7 +757,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -762,7 +765,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -770,7 +773,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -786,7 +789,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -794,7 +797,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -802,15 +805,15 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -818,7 +821,7 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -826,7 +829,7 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -834,7 +837,7 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -842,7 +845,7 @@
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -850,7 +853,7 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -858,7 +861,7 @@
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -866,7 +869,7 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -874,7 +877,7 @@
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -882,7 +885,7 @@
         <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -890,7 +893,7 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -914,7 +917,7 @@
         <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -922,7 +925,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -930,7 +933,7 @@
         <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -943,23 +946,23 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
         <v>3</v>
@@ -967,7 +970,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
@@ -975,7 +978,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
         <v>6</v>
@@ -983,31 +986,31 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
         <v>3</v>
@@ -1015,10 +1018,18 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>